<commit_message>
Add to comparison table
Former-commit-id: 31b6b598d3fc2e8468e95b8f372075c35f6f610f
</commit_message>
<xml_diff>
--- a/text/CRAN_Bayesian_spatial_point_process_review.xlsx
+++ b/text/CRAN_Bayesian_spatial_point_process_review.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seananderson/src/spatiotemporal-extremes/text/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="420" yWindow="0" windowWidth="25600" windowHeight="15800" tabRatio="500"/>
+    <workbookView xWindow="10500" yWindow="2580" windowWidth="30320" windowHeight="11220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="42">
   <si>
     <t>Package</t>
   </si>
@@ -30,12 +38,6 @@
     <t>spate</t>
   </si>
   <si>
-    <t>Simulation function?</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>Observation model</t>
   </si>
   <si>
@@ -48,15 +50,9 @@
     <t>ML Estimation</t>
   </si>
   <si>
-    <t>Cov functions</t>
-  </si>
-  <si>
     <t>Multivariate</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>spBayes</t>
   </si>
   <si>
@@ -69,9 +65,6 @@
     <t>MCMC</t>
   </si>
   <si>
-    <t>Exponential, Gaussian</t>
-  </si>
-  <si>
     <t>Gaussian, Binomial, Poisson</t>
   </si>
   <si>
@@ -90,9 +83,6 @@
     <t>https://github.com/James-Thorson/VAST</t>
   </si>
   <si>
-    <t>Site</t>
-  </si>
-  <si>
     <t>https://github.com/seananderson/rrfields</t>
   </si>
   <si>
@@ -136,6 +126,33 @@
   </si>
   <si>
     <t>http://www.r-inla.org/</t>
+  </si>
+  <si>
+    <t>Exponential, Gaussian, Matern family</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>MVT random fields</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Simulation function</t>
+  </si>
+  <si>
+    <t>Covariance functions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formula interface </t>
+  </si>
+  <si>
+    <t xml:space="preserve">?? </t>
   </si>
 </sst>
 </file>
@@ -191,8 +208,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -205,17 +224,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -541,259 +567,297 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>23</v>
+      <c r="L1" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="G2" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="I2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="J2" t="s">
-        <v>27</v>
+        <v>37</v>
+      </c>
+      <c r="K2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>28</v>
       </c>
-      <c r="H3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" t="s">
-        <v>26</v>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L7" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" t="s">
-        <v>4</v>
-      </c>
-      <c r="J4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J5" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>